<commit_message>
2709 +/- 13 Elo at bullet chess.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8F901-DD9E-4159-A45E-774C9654F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACBD2DA-2473-479A-AACB-7487654F530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="2130" windowWidth="29390" windowHeight="18290" activeTab="1" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
@@ -17528,7 +17528,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17552,13 +17552,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>200</v>
+        <v>128</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -17572,7 +17572,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -17580,13 +17580,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -17613,14 +17613,14 @@
       </c>
       <c r="B7" s="5">
         <f>$B$2 * POWER((A7 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
       <c r="E7" s="5">
         <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -17629,8 +17629,8 @@
         <v>800</v>
       </c>
       <c r="B8" s="5">
-        <f t="shared" ref="B8:B27" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>700</v>
+        <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
+        <v>160</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
@@ -17638,7 +17638,7 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ref="E8:E17" si="3">$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
-        <v>15</v>
+        <v>17.96</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -17648,7 +17648,7 @@
       </c>
       <c r="B9" s="5">
         <f t="shared" si="1"/>
-        <v>3700</v>
+        <v>2080</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
@@ -17656,7 +17656,7 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>15.24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -17666,7 +17666,7 @@
       </c>
       <c r="B10" s="5">
         <f t="shared" si="1"/>
-        <v>16700</v>
+        <v>10400</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
@@ -17674,7 +17674,7 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>12.84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -17684,7 +17684,7 @@
       </c>
       <c r="B11" s="5">
         <f t="shared" si="1"/>
-        <v>51700</v>
+        <v>32800</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
@@ -17692,7 +17692,7 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>10.76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -17702,7 +17702,7 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" si="1"/>
-        <v>125500</v>
+        <v>80032</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
@@ -17710,7 +17710,7 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -17720,7 +17720,7 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" si="1"/>
-        <v>259700</v>
+        <v>165920</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
@@ -17728,7 +17728,7 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.5600000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -17738,7 +17738,7 @@
       </c>
       <c r="B14" s="5">
         <f t="shared" si="1"/>
-        <v>480700</v>
+        <v>307360</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
@@ -17746,7 +17746,7 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>6.4399999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -17756,7 +17756,7 @@
       </c>
       <c r="B15" s="5">
         <f t="shared" si="1"/>
-        <v>819700</v>
+        <v>524320</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -17774,7 +17774,7 @@
       </c>
       <c r="B16" s="5">
         <f t="shared" si="1"/>
-        <v>1312700</v>
+        <v>839840</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
@@ -17782,7 +17782,7 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -17792,7 +17792,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" si="1"/>
-        <v>2000500</v>
+        <v>1280032</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
@@ -17800,7 +17800,7 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature/king safety improvements (#42)
* Committing changes before experimenting removing the _bestMoves array.

* Modified ScoredMovePriorityComparer to sort by score descending then priority descending.  Previously was sorting only by priority descending.  This guarantees the best move (or MultiPV best moves) at root are searched first even if the best move(s) were ejected from the cache.  Also improved MultiPV implementation by raising alpha to the MultiPvth best move's score.

* Experimented adding endgame king safety evaluation.  However, the particle swarm tuner left all EG KS eval params at or very near zero.  Removed EG KS evaluation.

* Added MgKingSafetyAttackingPiecesPer8 evaluation parameter.  Evaluates average distance of attacking pieces from enemy king.

* Testing engine strength.

* 2709 +/- 13 Elo at bullet chess.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8F901-DD9E-4159-A45E-774C9654F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACBD2DA-2473-479A-AACB-7487654F530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="2130" windowWidth="29390" windowHeight="18290" activeTab="1" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
@@ -17528,7 +17528,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17552,13 +17552,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>200</v>
+        <v>128</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -17572,7 +17572,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -17580,13 +17580,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -17613,14 +17613,14 @@
       </c>
       <c r="B7" s="5">
         <f>$B$2 * POWER((A7 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
       <c r="E7" s="5">
         <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -17629,8 +17629,8 @@
         <v>800</v>
       </c>
       <c r="B8" s="5">
-        <f t="shared" ref="B8:B27" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>700</v>
+        <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
+        <v>160</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
@@ -17638,7 +17638,7 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ref="E8:E17" si="3">$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
-        <v>15</v>
+        <v>17.96</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -17648,7 +17648,7 @@
       </c>
       <c r="B9" s="5">
         <f t="shared" si="1"/>
-        <v>3700</v>
+        <v>2080</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
@@ -17656,7 +17656,7 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>15.24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -17666,7 +17666,7 @@
       </c>
       <c r="B10" s="5">
         <f t="shared" si="1"/>
-        <v>16700</v>
+        <v>10400</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
@@ -17674,7 +17674,7 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>12.84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -17684,7 +17684,7 @@
       </c>
       <c r="B11" s="5">
         <f t="shared" si="1"/>
-        <v>51700</v>
+        <v>32800</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
@@ -17692,7 +17692,7 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>10.76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -17702,7 +17702,7 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" si="1"/>
-        <v>125500</v>
+        <v>80032</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
@@ -17710,7 +17710,7 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -17720,7 +17720,7 @@
       </c>
       <c r="B13" s="5">
         <f t="shared" si="1"/>
-        <v>259700</v>
+        <v>165920</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
@@ -17728,7 +17728,7 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.5600000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -17738,7 +17738,7 @@
       </c>
       <c r="B14" s="5">
         <f t="shared" si="1"/>
-        <v>480700</v>
+        <v>307360</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
@@ -17746,7 +17746,7 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>6.4399999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -17756,7 +17756,7 @@
       </c>
       <c r="B15" s="5">
         <f t="shared" si="1"/>
-        <v>819700</v>
+        <v>524320</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -17774,7 +17774,7 @@
       </c>
       <c r="B16" s="5">
         <f t="shared" si="1"/>
-        <v>1312700</v>
+        <v>839840</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
@@ -17782,7 +17782,7 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -17792,7 +17792,7 @@
       </c>
       <c r="B17" s="5">
         <f t="shared" si="1"/>
-        <v>2000500</v>
+        <v>1280032</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
@@ -17800,7 +17800,7 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2712 +/- 13 Elo at bullet chess.  Adjusted futility pruning and late move pruning margins.  Use non-linear equation for margin at specified toHorizon.  Limit margins to a maximum toHorizon of 7.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E211742-968C-48ED-ADDE-3EAA9E6CBF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CB99E9-7948-4EC2-8805-3F690B5ABB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4650" yWindow="1470" windowWidth="29390" windowHeight="18290" activeTab="2" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
@@ -143,9 +143,10 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -153,10 +154,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,31 +483,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>1</v>
       </c>
@@ -765,10 +765,10 @@
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="3">
         <v>1</v>
       </c>
@@ -17562,14 +17562,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -17842,53 +17842,52 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14">
-        <f>1/4</f>
-        <v>0.25</v>
+      <c r="E1" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
-        <f>($E$1 * POWER(A2, $E$2)) + $E$3</f>
-        <v>3.25</v>
+      <c r="B2" s="9">
+        <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E2">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f>A2 + 1</f>
+        <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="13">
-        <f>($E$1 * POWER(A3, $E$2)) + $E$3</f>
-        <v>4.4142135623730949</v>
+      <c r="B3" s="9">
+        <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -17899,72 +17898,72 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f>A3 + 1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="13">
-        <f>($E$1 * POWER(A4, $E$2)) + $E$3</f>
-        <v>6.8971143170299758</v>
+      <c r="B4" s="9">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <f>A4 + 1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="13">
-        <f>($E$1 * POWER(A5, $E$2)) + $E$3</f>
-        <v>11</v>
+      <c r="B5" s="9">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f>A5 + 1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="13">
-        <f>($E$1 * POWER(A6, $E$2)) + $E$3</f>
-        <v>16.975424859373682</v>
+      <c r="B6" s="9">
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <f>A6 + 1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="13">
-        <f>($E$1 * POWER(A7, $E$2)) + $E$3</f>
-        <v>25.045407685048595</v>
+      <c r="B7" s="9">
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f>A7 + 1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="13">
-        <f>($E$1 * POWER(A8, $E$2)) + $E$3</f>
-        <v>35.410453560541221</v>
+      <c r="B8" s="9">
+        <f t="shared" si="1"/>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f>A8 + 1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="13">
-        <f>($E$1 * POWER(A9, $E$2)) + $E$3</f>
-        <v>48.25483399593903</v>
+      <c r="B9" s="9">
+        <f t="shared" si="1"/>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f>A9 + 1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="13">
-        <f>($E$1 * POWER(A10, $E$2)) + $E$3</f>
-        <v>63.750000000000043</v>
+      <c r="B10" s="9">
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In Cache class, round indices up to nearest power of two to enable fast modular division in GetIndex method.  Fixed bug in particle swam optimizer that prevented initializing all particles to a random location in parameter-space (they all started at best known location).  Tuned evaluation parameters against games from MadChessGauntlets.pgn database.  Initialized all particles to a random location in parameter-space.  After two days the partical swarm optimizer found a set a parameters with slightly less error than previously found.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CB99E9-7948-4EC2-8805-3F690B5ABB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F907148-D45C-488E-8A08-F64201059093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="29390" windowHeight="18290" activeTab="2" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
+    <workbookView xWindow="4650" yWindow="1470" windowWidth="29390" windowHeight="18290" activeTab="3" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="LateMoveReductions" sheetId="2" r:id="rId1"/>
     <sheet name="LimitStrength" sheetId="3" r:id="rId2"/>
     <sheet name="LateMovePruning" sheetId="4" r:id="rId3"/>
+    <sheet name="Tuning Sigmoid" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Quiet Move Number</t>
   </si>
@@ -76,6 +77,15 @@
   </si>
   <si>
     <t>QuietMoveNumber</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Win Fraction</t>
+  </si>
+  <si>
+    <t>Win Scale</t>
   </si>
 </sst>
 </file>
@@ -135,10 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -147,7 +156,13 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -156,6 +171,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,298 +499,295 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="16384" width="8.7265625" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="2">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="2">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="3">
+      <c r="C4" s="13"/>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>D4 + 1</f>
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>E4 + 1</f>
         <v>3</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>F4 + 1</f>
         <v>4</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f t="shared" ref="H4:BO4" si="0">G4 + 1</f>
         <v>5</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="Z4" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA4" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AC4" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AD4" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AE4" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AF4" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AG4" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AH4" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AI4" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AJ4" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AK4" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AL4" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AM4" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AN4" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AO4" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AP4" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AQ4" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AR4" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AS4" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AT4" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AU4" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AV4" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AW4" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AX4" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AY4" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="AZ4" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BA4" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BB4" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BC4" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BD4" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BE4" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BF4" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BG4" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BH4" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BI4" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BJ4" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BK4" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BL4" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BM4" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BN4" s="3">
+      <c r="BN4" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BO4" s="3">
+      <c r="BO4" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="1">
@@ -1030,7 +1048,7 @@
       </c>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f>C5 + 1</f>
         <v>2</v>
       </c>
@@ -1292,7 +1310,7 @@
       </c>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f>C6 + 1</f>
         <v>3</v>
       </c>
@@ -1554,7 +1572,7 @@
       </c>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>C7 + 1</f>
         <v>4</v>
       </c>
@@ -1816,7 +1834,7 @@
       </c>
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" ref="C9:C68" si="3">C8 + 1</f>
         <v>5</v>
       </c>
@@ -2078,7 +2096,7 @@
       </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -2340,7 +2358,7 @@
       </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -2602,7 +2620,7 @@
       </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -2864,7 +2882,7 @@
       </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3126,7 +3144,7 @@
       </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3388,7 +3406,7 @@
       </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3650,7 +3668,7 @@
       </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3912,7 +3930,7 @@
       </c>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
@@ -4174,7 +4192,7 @@
       </c>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
@@ -4436,7 +4454,7 @@
       </c>
     </row>
     <row r="19" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
@@ -4698,7 +4716,7 @@
       </c>
     </row>
     <row r="20" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -4960,7 +4978,7 @@
       </c>
     </row>
     <row r="21" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
@@ -5222,7 +5240,7 @@
       </c>
     </row>
     <row r="22" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -5484,7 +5502,7 @@
       </c>
     </row>
     <row r="23" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
@@ -5746,7 +5764,7 @@
       </c>
     </row>
     <row r="24" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -6008,7 +6026,7 @@
       </c>
     </row>
     <row r="25" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
@@ -6270,7 +6288,7 @@
       </c>
     </row>
     <row r="26" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -6532,7 +6550,7 @@
       </c>
     </row>
     <row r="27" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
@@ -6794,7 +6812,7 @@
       </c>
     </row>
     <row r="28" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
@@ -7056,7 +7074,7 @@
       </c>
     </row>
     <row r="29" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
@@ -7318,7 +7336,7 @@
       </c>
     </row>
     <row r="30" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -7580,7 +7598,7 @@
       </c>
     </row>
     <row r="31" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
@@ -7842,7 +7860,7 @@
       </c>
     </row>
     <row r="32" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
@@ -8104,7 +8122,7 @@
       </c>
     </row>
     <row r="33" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
@@ -8366,7 +8384,7 @@
       </c>
     </row>
     <row r="34" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -8628,7 +8646,7 @@
       </c>
     </row>
     <row r="35" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
@@ -8890,7 +8908,7 @@
       </c>
     </row>
     <row r="36" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
@@ -9152,7 +9170,7 @@
       </c>
     </row>
     <row r="37" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
@@ -9414,7 +9432,7 @@
       </c>
     </row>
     <row r="38" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
@@ -9676,7 +9694,7 @@
       </c>
     </row>
     <row r="39" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
@@ -9938,7 +9956,7 @@
       </c>
     </row>
     <row r="40" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
@@ -10200,7 +10218,7 @@
       </c>
     </row>
     <row r="41" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
@@ -10462,7 +10480,7 @@
       </c>
     </row>
     <row r="42" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -10724,7 +10742,7 @@
       </c>
     </row>
     <row r="43" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -10986,7 +11004,7 @@
       </c>
     </row>
     <row r="44" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
@@ -11248,7 +11266,7 @@
       </c>
     </row>
     <row r="45" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
@@ -11510,7 +11528,7 @@
       </c>
     </row>
     <row r="46" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
@@ -11772,7 +11790,7 @@
       </c>
     </row>
     <row r="47" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
@@ -12034,7 +12052,7 @@
       </c>
     </row>
     <row r="48" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
@@ -12296,7 +12314,7 @@
       </c>
     </row>
     <row r="49" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
@@ -12558,7 +12576,7 @@
       </c>
     </row>
     <row r="50" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
@@ -12820,7 +12838,7 @@
       </c>
     </row>
     <row r="51" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
@@ -13082,7 +13100,7 @@
       </c>
     </row>
     <row r="52" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
@@ -13344,7 +13362,7 @@
       </c>
     </row>
     <row r="53" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
@@ -13606,7 +13624,7 @@
       </c>
     </row>
     <row r="54" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
@@ -13868,7 +13886,7 @@
       </c>
     </row>
     <row r="55" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
@@ -14130,7 +14148,7 @@
       </c>
     </row>
     <row r="56" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
@@ -14392,7 +14410,7 @@
       </c>
     </row>
     <row r="57" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
@@ -14654,7 +14672,7 @@
       </c>
     </row>
     <row r="58" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
@@ -14916,7 +14934,7 @@
       </c>
     </row>
     <row r="59" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C59" s="3">
+      <c r="C59" s="2">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
@@ -15178,7 +15196,7 @@
       </c>
     </row>
     <row r="60" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
@@ -15440,7 +15458,7 @@
       </c>
     </row>
     <row r="61" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
@@ -15702,7 +15720,7 @@
       </c>
     </row>
     <row r="62" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C62" s="3">
+      <c r="C62" s="2">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
@@ -15964,7 +15982,7 @@
       </c>
     </row>
     <row r="63" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
@@ -16226,7 +16244,7 @@
       </c>
     </row>
     <row r="64" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
@@ -16488,7 +16506,7 @@
       </c>
     </row>
     <row r="65" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C65" s="3">
+      <c r="C65" s="2">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
@@ -16750,7 +16768,7 @@
       </c>
     </row>
     <row r="66" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C66" s="3">
+      <c r="C66" s="2">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
@@ -17012,7 +17030,7 @@
       </c>
     </row>
     <row r="67" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C67" s="3">
+      <c r="C67" s="2">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
@@ -17274,7 +17292,7 @@
       </c>
     </row>
     <row r="68" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
@@ -17562,72 +17580,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>128</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>32</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -17635,14 +17653,14 @@
       <c r="A7">
         <v>600</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>$B$2 * POWER((A7 - $A$7) / 200, $B$3) +$B$4</f>
         <v>32</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
         <v>21</v>
       </c>
@@ -17652,7 +17670,7 @@
         <f t="shared" ref="A8:A17" si="0">A7 + 200</f>
         <v>800</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
         <v>160</v>
       </c>
@@ -17660,7 +17678,7 @@
         <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
         <v>800</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" ref="E8:E17" si="3">$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
         <v>17.96</v>
       </c>
@@ -17670,7 +17688,7 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <f t="shared" si="1"/>
         <v>2080</v>
       </c>
@@ -17678,7 +17696,7 @@
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f t="shared" si="3"/>
         <v>15.24</v>
       </c>
@@ -17688,7 +17706,7 @@
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <f t="shared" si="1"/>
         <v>10400</v>
       </c>
@@ -17696,7 +17714,7 @@
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="3"/>
         <v>12.84</v>
       </c>
@@ -17706,7 +17724,7 @@
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <f t="shared" si="1"/>
         <v>32800</v>
       </c>
@@ -17714,7 +17732,7 @@
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="3"/>
         <v>10.76</v>
       </c>
@@ -17724,7 +17742,7 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <f t="shared" si="1"/>
         <v>80032</v>
       </c>
@@ -17732,7 +17750,7 @@
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -17742,7 +17760,7 @@
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f t="shared" si="1"/>
         <v>165920</v>
       </c>
@@ -17750,7 +17768,7 @@
         <f t="shared" si="2"/>
         <v>1800</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="3"/>
         <v>7.5600000000000005</v>
       </c>
@@ -17760,7 +17778,7 @@
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f t="shared" si="1"/>
         <v>307360</v>
       </c>
@@ -17768,7 +17786,7 @@
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="3"/>
         <v>6.4399999999999995</v>
       </c>
@@ -17778,7 +17796,7 @@
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f t="shared" si="1"/>
         <v>524320</v>
       </c>
@@ -17786,7 +17804,7 @@
         <f t="shared" si="2"/>
         <v>2200</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="3"/>
         <v>5.64</v>
       </c>
@@ -17796,7 +17814,7 @@
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f t="shared" si="1"/>
         <v>839840</v>
       </c>
@@ -17804,7 +17822,7 @@
         <f t="shared" si="2"/>
         <v>2400</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f t="shared" si="3"/>
         <v>5.16</v>
       </c>
@@ -17814,7 +17832,7 @@
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <f t="shared" si="1"/>
         <v>1280032</v>
       </c>
@@ -17822,7 +17840,7 @@
         <f t="shared" si="2"/>
         <v>2600</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -17841,27 +17859,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10">
+      <c r="E1" s="9">
         <v>1</v>
       </c>
     </row>
@@ -17869,11 +17887,11 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2">
@@ -17885,11 +17903,11 @@
         <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3">
@@ -17901,7 +17919,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -17911,7 +17929,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -17921,7 +17939,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -17931,7 +17949,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
@@ -17941,7 +17959,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
@@ -17951,7 +17969,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
@@ -17961,7 +17979,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
@@ -17970,4 +17988,207 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D75E8BC-3113-4D5F-9721-2C5404FEE815}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.08984375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>800</v>
+      </c>
+      <c r="B2" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A2 / $D$2)))</f>
+        <v>0.96055077075785666</v>
+      </c>
+      <c r="D2" s="11">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <f>A2 - 100</f>
+        <v>700</v>
+      </c>
+      <c r="B3" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A3 / $D$2)))</f>
+        <v>0.94231980226632672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <f t="shared" ref="A4:A18" si="0">A3 - 100</f>
+        <v>600</v>
+      </c>
+      <c r="B4" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A4 / $D$2)))</f>
+        <v>0.91639692148646656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="B5" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A5 / $D$2)))</f>
+        <v>0.88030353627105185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="B6" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A6 / $D$2)))</f>
+        <v>0.83149308082614892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="B7" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A7 / $D$2)))</f>
+        <v>0.76802356512493686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="B8" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A8 / $D$2)))</f>
+        <v>0.68957284718215062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="B9" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A9 / $D$2)))</f>
+        <v>0.59846216444498745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A10 / $D$2)))</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="B11" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A11 / $D$2)))</f>
+        <v>0.4015378355550126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <f t="shared" si="0"/>
+        <v>-200</v>
+      </c>
+      <c r="B12" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A12 / $D$2)))</f>
+        <v>0.31042715281784933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <f t="shared" si="0"/>
+        <v>-300</v>
+      </c>
+      <c r="B13" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A13 / $D$2)))</f>
+        <v>0.23197643487506323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <f t="shared" si="0"/>
+        <v>-400</v>
+      </c>
+      <c r="B14" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A14 / $D$2)))</f>
+        <v>0.16850691917385111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <f t="shared" si="0"/>
+        <v>-500</v>
+      </c>
+      <c r="B15" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A15 / $D$2)))</f>
+        <v>0.11969646372894807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <f t="shared" si="0"/>
+        <v>-600</v>
+      </c>
+      <c r="B16" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A16 / $D$2)))</f>
+        <v>8.3603078513533449E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="B17" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A17 / $D$2)))</f>
+        <v>5.7680197733673291E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <f t="shared" si="0"/>
+        <v>-800</v>
+      </c>
+      <c r="B18" s="17">
+        <f>1 / (1 + POWER(10, (-1 * A18 / $D$2)))</f>
+        <v>3.9449229242143363E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusted limit-strength parameters in Search.ConfigureLimitedStrength method.  Made engine less prone to blundering pieces.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F907148-D45C-488E-8A08-F64201059093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F997392-B05E-463E-A510-9A6F5700775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="29390" windowHeight="18290" activeTab="3" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
+    <workbookView xWindow="3000" yWindow="1550" windowWidth="29390" windowHeight="18290" activeTab="1" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="LateMoveReductions" sheetId="2" r:id="rId1"/>
     <sheet name="LimitStrength" sheetId="3" r:id="rId2"/>
-    <sheet name="LateMovePruning" sheetId="4" r:id="rId3"/>
-    <sheet name="Tuning Sigmoid" sheetId="5" r:id="rId4"/>
+    <sheet name="Futility Pruning" sheetId="6" r:id="rId3"/>
+    <sheet name="LateMovePruning" sheetId="4" r:id="rId4"/>
+    <sheet name="Tuning Sigmoid" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Quiet Move Number</t>
   </si>
@@ -67,12 +68,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Scale Up</t>
-  </si>
-  <si>
-    <t>Scale Down</t>
-  </si>
-  <si>
     <t>ToHorizon</t>
   </si>
   <si>
@@ -87,13 +82,31 @@
   <si>
     <t>Win Scale</t>
   </si>
+  <si>
+    <t>Nodes Per Second</t>
+  </si>
+  <si>
+    <t>Move Error</t>
+  </si>
+  <si>
+    <t>Blunder Error</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Blunder Per 128</t>
+  </si>
+  <si>
+    <t>Moves Until Blunder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -145,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -155,11 +168,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -172,12 +190,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,31 +515,31 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -783,10 +797,10 @@
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -17567,43 +17581,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79230DCC-5E5F-492F-8E29-85439474ACBD}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="13.6328125" customWidth="1"/>
     <col min="4" max="5" width="13.6328125" customWidth="1"/>
+    <col min="7" max="8" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="8"/>
+    <col min="13" max="13" width="18.1796875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="D1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="15"/>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3">
         <v>0.16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -17616,8 +17654,20 @@
       <c r="E3" s="3">
         <v>2</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -17630,12 +17680,26 @@
       <c r="E4" s="3">
         <v>5</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="E5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -17648,8 +17712,26 @@
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>600</v>
       </c>
@@ -17662,193 +17744,457 @@
       </c>
       <c r="E7" s="4">
         <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
+        <v>55</v>
+      </c>
+      <c r="G7">
+        <v>600</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$H$2 * POWER(($G$17 - G7) / 200, $H$3) +$H$4</f>
+        <v>341.22776601683825</v>
+      </c>
+      <c r="J7">
+        <v>600</v>
+      </c>
+      <c r="K7" s="4">
+        <f>$K$2 * POWER((J$17 - J7) / 200, $K$3) +$K$4</f>
         <v>21</v>
       </c>
+      <c r="L7" s="8">
+        <f>(K7 *100) / 128</f>
+        <v>16.40625</v>
+      </c>
+      <c r="M7" s="17">
+        <f xml:space="preserve"> 128 / K7</f>
+        <v>6.0952380952380949</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ref="A8:A17" si="0">A7 + 200</f>
         <v>800</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>160</v>
+        <v>224</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
         <v>800</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" ref="E8:E17" si="3">$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
+        <f>$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
+        <v>45.5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G17" si="3">G7 + 200</f>
+        <v>800</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$H$2 * POWER(($G$17 - G8) / 200, $H$3) +$H$4</f>
+        <v>268.00000000000017</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J17" si="4">J7 + 200</f>
+        <v>800</v>
+      </c>
+      <c r="K8" s="4">
+        <f>$K$2 * POWER((J$17 - J8) / 200, $K$3) +$K$4</f>
         <v>17.96</v>
       </c>
+      <c r="L8" s="8">
+        <f t="shared" ref="L8:L17" si="5">(K8 *100) / 128</f>
+        <v>14.03125</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" ref="M8:M17" si="6" xml:space="preserve"> 128 / K8</f>
+        <v>7.1269487750556788</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="1"/>
-        <v>2080</v>
+        <v>3104</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="E9" s="4">
+        <f>$E$2 * POWER(($D$17 - D9) / 200, $E$3) +$E$4</f>
+        <v>37</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$H$2 * POWER(($G$17 - G9) / 200, $H$3) +$H$4</f>
+        <v>206.01933598375612</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="K9" s="4">
+        <f>$K$2 * POWER((J$17 - J9) / 200, $K$3) +$K$4</f>
         <v>15.24</v>
       </c>
+      <c r="L9" s="8">
+        <f t="shared" si="5"/>
+        <v>11.90625</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="6"/>
+        <v>8.3989501312335957</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="1"/>
-        <v>10400</v>
+        <v>15584</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="E10" s="4">
+        <f>$E$2 * POWER(($D$17 - D10) / 200, $E$3) +$E$4</f>
+        <v>29.5</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$H$2 * POWER(($G$17 - G10) / 200, $H$3) +$H$4</f>
+        <v>154.64181424216488</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="K10" s="4">
+        <f>$K$2 * POWER((J$17 - J10) / 200, $K$3) +$K$4</f>
         <v>12.84</v>
       </c>
+      <c r="L10" s="8">
+        <f t="shared" si="5"/>
+        <v>10.03125</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="6"/>
+        <v>9.9688473520249214</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="1"/>
-        <v>32800</v>
+        <v>49184</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="E11" s="4">
+        <f>$E$2 * POWER(($D$17 - D11) / 200, $E$3) +$E$4</f>
+        <v>23</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="3"/>
+        <v>1400</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$H$2 * POWER(($G$17 - G11) / 200, $H$3) +$H$4</f>
+        <v>113.18163074019438</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>1400</v>
+      </c>
+      <c r="K11" s="4">
+        <f>$K$2 * POWER((J$17 - J11) / 200, $K$3) +$K$4</f>
         <v>10.76</v>
       </c>
+      <c r="L11" s="8">
+        <f t="shared" si="5"/>
+        <v>8.40625</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="6"/>
+        <v>11.895910780669146</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="1"/>
-        <v>80032</v>
+        <v>120032</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="E12" s="4">
+        <f>$E$2 * POWER(($D$17 - D12) / 200, $E$3) +$E$4</f>
+        <v>17.5</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="3"/>
+        <v>1600</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$H$2 * POWER(($G$17 - G12) / 200, $H$3) +$H$4</f>
+        <v>80.901699437494727</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>1600</v>
+      </c>
+      <c r="K12" s="4">
+        <f>$K$2 * POWER((J$17 - J12) / 200, $K$3) +$K$4</f>
         <v>9</v>
       </c>
+      <c r="L12" s="8">
+        <f t="shared" si="5"/>
+        <v>7.03125</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="6"/>
+        <v>14.222222222222221</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="1"/>
-        <v>165920</v>
+        <v>248864</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="E13" s="4">
+        <f>$E$2 * POWER(($D$17 - D13) / 200, $E$3) +$E$4</f>
+        <v>13</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$H$2 * POWER(($G$17 - G13) / 200, $H$3) +$H$4</f>
+        <v>57</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>1800</v>
+      </c>
+      <c r="K13" s="4">
+        <f>$K$2 * POWER((J$17 - J13) / 200, $K$3) +$K$4</f>
         <v>7.5600000000000005</v>
       </c>
+      <c r="L13" s="8">
+        <f t="shared" si="5"/>
+        <v>5.90625</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="6"/>
+        <v>16.93121693121693</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="1"/>
-        <v>307360</v>
+        <v>461024</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="E14" s="4">
+        <f>$E$2 * POWER(($D$17 - D14) / 200, $E$3) +$E$4</f>
+        <v>9.5</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="H14" s="4">
+        <f>$H$2 * POWER(($G$17 - G14) / 200, $H$3) +$H$4</f>
+        <v>40.588457268119903</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="K14" s="4">
+        <f>$K$2 * POWER((J$17 - J14) / 200, $K$3) +$K$4</f>
         <v>6.4399999999999995</v>
       </c>
+      <c r="L14" s="8">
+        <f t="shared" si="5"/>
+        <v>5.03125</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" si="6"/>
+        <v>19.87577639751553</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="1"/>
-        <v>524320</v>
+        <v>786464</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="E15" s="4">
+        <f>$E$2 * POWER(($D$17 - D15) / 200, $E$3) +$E$4</f>
+        <v>7</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$H$2 * POWER(($G$17 - G15) / 200, $H$3) +$H$4</f>
+        <v>30.65685424949238</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>2200</v>
+      </c>
+      <c r="K15" s="4">
+        <f>$K$2 * POWER((J$17 - J15) / 200, $K$3) +$K$4</f>
         <v>5.64</v>
       </c>
+      <c r="L15" s="8">
+        <f t="shared" si="5"/>
+        <v>4.40625</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" si="6"/>
+        <v>22.695035460992909</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f>A15 + 200</f>
         <v>2400</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="1"/>
-        <v>839840</v>
+        <v>1259744</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f>D15 + 200</f>
         <v>2400</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="3"/>
+        <f>$E$2 * POWER(($D$17 - D16) / 200, $E$3) +$E$4</f>
+        <v>5.5</v>
+      </c>
+      <c r="G16">
+        <f>G15 + 200</f>
+        <v>2400</v>
+      </c>
+      <c r="H16" s="4">
+        <f>$H$2 * POWER(($G$17 - G16) / 200, $H$3) +$H$4</f>
+        <v>26</v>
+      </c>
+      <c r="J16">
+        <f>J15 + 200</f>
+        <v>2400</v>
+      </c>
+      <c r="K16" s="4">
+        <f>$K$2 * POWER((J$17 - J16) / 200, $K$3) +$K$4</f>
         <v>5.16</v>
       </c>
+      <c r="L16" s="8">
+        <f t="shared" si="5"/>
+        <v>4.03125</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" si="6"/>
+        <v>24.806201550387595</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
       <c r="B17" s="4">
         <f t="shared" si="1"/>
-        <v>1280032</v>
+        <v>1920032</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
         <v>2600</v>
       </c>
       <c r="E17" s="4">
+        <f>$E$2 * POWER(($D$17 - D17) / 200, $E$3) +$E$4</f>
+        <v>5</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="H17" s="4">
+        <f>$H$2 * POWER(($G$17 - G17) / 200, $H$3) +$H$4</f>
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>2600</v>
+      </c>
+      <c r="K17" s="4">
+        <f>$K$2 * POWER((J$17 - J17) / 200, $K$3) +$K$4</f>
         <v>5</v>
+      </c>
+      <c r="L17" s="8">
+        <f t="shared" si="5"/>
+        <v>3.90625</v>
+      </c>
+      <c r="M17" s="17">
+        <f t="shared" si="6"/>
+        <v>25.6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17856,31 +18202,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4CD39-04D6-4A1F-9AA8-46EE1D516721}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9">
-        <v>1</v>
+      <c r="E1" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -17889,12 +18236,12 @@
       </c>
       <c r="B2" s="8">
         <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
     </row>
@@ -17905,13 +18252,13 @@
       </c>
       <c r="B3" s="8">
         <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>3</v>
+      <c r="E3" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -17921,7 +18268,7 @@
       </c>
       <c r="B4" s="8">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -17931,7 +18278,7 @@
       </c>
       <c r="B5" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -17941,7 +18288,7 @@
       </c>
       <c r="B6" s="8">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -17951,7 +18298,7 @@
       </c>
       <c r="B7" s="8">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>626</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -17961,7 +18308,7 @@
       </c>
       <c r="B8" s="8">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>834</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -17971,7 +18318,7 @@
       </c>
       <c r="B9" s="8">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -17981,7 +18328,7 @@
       </c>
       <c r="B10" s="8">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
@@ -17991,200 +18338,336 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D75E8BC-3113-4D5F-9721-2C5404FEE815}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>800</v>
       </c>
-      <c r="B2" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A2 / $D$2)))</f>
+      <c r="B2" s="12">
+        <f t="shared" ref="B2:B18" si="0">1 / (1 + POWER(10, (-1 * A2 / $D$2)))</f>
         <v>0.96055077075785666</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>577</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <f>A2 - 100</f>
         <v>700</v>
       </c>
-      <c r="B3" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A3 / $D$2)))</f>
+      <c r="B3" s="12">
+        <f t="shared" si="0"/>
         <v>0.94231980226632672</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
-        <f t="shared" ref="A4:A18" si="0">A3 - 100</f>
+      <c r="A4" s="10">
+        <f t="shared" ref="A4:A18" si="1">A3 - 100</f>
         <v>600</v>
       </c>
-      <c r="B4" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A4 / $D$2)))</f>
+      <c r="B4" s="12">
+        <f t="shared" si="0"/>
         <v>0.91639692148646656</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="B5" s="12">
         <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="B5" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A5 / $D$2)))</f>
         <v>0.88030353627105185</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="B6" s="12">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="B6" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A6 / $D$2)))</f>
         <v>0.83149308082614892</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="B7" s="12">
         <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="B7" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A7 / $D$2)))</f>
         <v>0.76802356512493686</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="B8" s="12">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="B8" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A8 / $D$2)))</f>
         <v>0.68957284718215062</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B9" s="12">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="B9" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A9 / $D$2)))</f>
         <v>0.59846216444498745</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B10" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A10 / $D$2)))</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>-100</v>
-      </c>
-      <c r="B11" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A11 / $D$2)))</f>
         <v>0.4015378355550126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="B12" s="12">
         <f t="shared" si="0"/>
-        <v>-200</v>
-      </c>
-      <c r="B12" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A12 / $D$2)))</f>
         <v>0.31042715281784933</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
+        <f t="shared" si="1"/>
+        <v>-300</v>
+      </c>
+      <c r="B13" s="12">
         <f t="shared" si="0"/>
-        <v>-300</v>
-      </c>
-      <c r="B13" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A13 / $D$2)))</f>
         <v>0.23197643487506323</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
+        <f t="shared" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="B14" s="12">
         <f t="shared" si="0"/>
-        <v>-400</v>
-      </c>
-      <c r="B14" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A14 / $D$2)))</f>
         <v>0.16850691917385111</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="B15" s="12">
         <f t="shared" si="0"/>
-        <v>-500</v>
-      </c>
-      <c r="B15" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A15 / $D$2)))</f>
         <v>0.11969646372894807</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
+        <f t="shared" si="1"/>
+        <v>-600</v>
+      </c>
+      <c r="B16" s="12">
         <f t="shared" si="0"/>
-        <v>-600</v>
-      </c>
-      <c r="B16" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A16 / $D$2)))</f>
         <v>8.3603078513533449E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
+        <f t="shared" si="1"/>
+        <v>-700</v>
+      </c>
+      <c r="B17" s="12">
         <f t="shared" si="0"/>
-        <v>-700</v>
-      </c>
-      <c r="B17" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A17 / $D$2)))</f>
         <v>5.7680197733673291E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
+        <f t="shared" si="1"/>
+        <v>-800</v>
+      </c>
+      <c r="B18" s="12">
         <f t="shared" si="0"/>
-        <v>-800</v>
-      </c>
-      <c r="B18" s="17">
-        <f>1 / (1 + POWER(10, (-1 * A18 / $D$2)))</f>
         <v>3.9449229242143363E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature/tune eval params (#48)
* In Cache class, round indices up to nearest power of two to enable fast modular division in GetIndex method.  Fixed bug in particle swam optimizer that prevented initializing all particles to a random location in parameter-space (they all started at best known location).  Tuned evaluation parameters against games from MadChessGauntlets.pgn database.  Initialized all particles to a random location in parameter-space.  After two days the partical swarm optimizer found a set a parameters with slightly less error than previously found.

* 2714 +/- 14 Elo at bullet chess.

* 2709 +/- 13 Elo at bullet chess.

* 2729 +/- 13 Elo at bullet chess.

* Updated bullet rating list.

* Reformatted one-liner for loops as two lines.

* Adjusted limit-strength parameters in Search.ConfigureLimitedStrength method.  Made engine less prone to blundering pieces.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CB99E9-7948-4EC2-8805-3F690B5ABB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F997392-B05E-463E-A510-9A6F5700775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="1470" windowWidth="29390" windowHeight="18290" activeTab="2" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
+    <workbookView xWindow="3000" yWindow="1550" windowWidth="29390" windowHeight="18290" activeTab="1" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="LateMoveReductions" sheetId="2" r:id="rId1"/>
     <sheet name="LimitStrength" sheetId="3" r:id="rId2"/>
-    <sheet name="LateMovePruning" sheetId="4" r:id="rId3"/>
+    <sheet name="Futility Pruning" sheetId="6" r:id="rId3"/>
+    <sheet name="LateMovePruning" sheetId="4" r:id="rId4"/>
+    <sheet name="Tuning Sigmoid" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Quiet Move Number</t>
   </si>
@@ -66,16 +68,37 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Scale Up</t>
-  </si>
-  <si>
-    <t>Scale Down</t>
-  </si>
-  <si>
     <t>ToHorizon</t>
   </si>
   <si>
     <t>QuietMoveNumber</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Win Fraction</t>
+  </si>
+  <si>
+    <t>Win Scale</t>
+  </si>
+  <si>
+    <t>Nodes Per Second</t>
+  </si>
+  <si>
+    <t>Move Error</t>
+  </si>
+  <si>
+    <t>Blunder Error</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Blunder Per 128</t>
+  </si>
+  <si>
+    <t>Moves Until Blunder</t>
   </si>
 </sst>
 </file>
@@ -83,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -135,10 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -146,8 +168,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -157,6 +190,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,298 +513,295 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="16384" width="8.7265625" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="2">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="2">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="3">
+      <c r="C4" s="14"/>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>D4 + 1</f>
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>E4 + 1</f>
         <v>3</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>F4 + 1</f>
         <v>4</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f t="shared" ref="H4:BO4" si="0">G4 + 1</f>
         <v>5</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="Z4" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA4" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AC4" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AD4" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AE4" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AF4" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AG4" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AH4" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AI4" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AJ4" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AK4" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AL4" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AM4" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AN4" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AO4" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AP4" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AQ4" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AR4" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AS4" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AT4" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AU4" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AV4" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AW4" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AX4" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AY4" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="AZ4" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BA4" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BB4" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BC4" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BD4" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BE4" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BF4" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BG4" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BH4" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BI4" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BJ4" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BK4" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BL4" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BM4" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BN4" s="3">
+      <c r="BN4" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BO4" s="3">
+      <c r="BO4" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="3">
+      <c r="B5" s="15"/>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="1">
@@ -1030,7 +1062,7 @@
       </c>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <f>C5 + 1</f>
         <v>2</v>
       </c>
@@ -1292,7 +1324,7 @@
       </c>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f>C6 + 1</f>
         <v>3</v>
       </c>
@@ -1554,7 +1586,7 @@
       </c>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>C7 + 1</f>
         <v>4</v>
       </c>
@@ -1816,7 +1848,7 @@
       </c>
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" ref="C9:C68" si="3">C8 + 1</f>
         <v>5</v>
       </c>
@@ -2078,7 +2110,7 @@
       </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -2340,7 +2372,7 @@
       </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -2602,7 +2634,7 @@
       </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -2864,7 +2896,7 @@
       </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -3126,7 +3158,7 @@
       </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3388,7 +3420,7 @@
       </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3650,7 +3682,7 @@
       </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3912,7 +3944,7 @@
       </c>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
@@ -4174,7 +4206,7 @@
       </c>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
@@ -4436,7 +4468,7 @@
       </c>
     </row>
     <row r="19" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
@@ -4698,7 +4730,7 @@
       </c>
     </row>
     <row r="20" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -4960,7 +4992,7 @@
       </c>
     </row>
     <row r="21" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
@@ -5222,7 +5254,7 @@
       </c>
     </row>
     <row r="22" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -5484,7 +5516,7 @@
       </c>
     </row>
     <row r="23" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
@@ -5746,7 +5778,7 @@
       </c>
     </row>
     <row r="24" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -6008,7 +6040,7 @@
       </c>
     </row>
     <row r="25" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
@@ -6270,7 +6302,7 @@
       </c>
     </row>
     <row r="26" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -6532,7 +6564,7 @@
       </c>
     </row>
     <row r="27" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
@@ -6794,7 +6826,7 @@
       </c>
     </row>
     <row r="28" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
@@ -7056,7 +7088,7 @@
       </c>
     </row>
     <row r="29" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
@@ -7318,7 +7350,7 @@
       </c>
     </row>
     <row r="30" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -7580,7 +7612,7 @@
       </c>
     </row>
     <row r="31" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
@@ -7842,7 +7874,7 @@
       </c>
     </row>
     <row r="32" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
@@ -8104,7 +8136,7 @@
       </c>
     </row>
     <row r="33" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
@@ -8366,7 +8398,7 @@
       </c>
     </row>
     <row r="34" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -8628,7 +8660,7 @@
       </c>
     </row>
     <row r="35" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
@@ -8890,7 +8922,7 @@
       </c>
     </row>
     <row r="36" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
@@ -9152,7 +9184,7 @@
       </c>
     </row>
     <row r="37" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
@@ -9414,7 +9446,7 @@
       </c>
     </row>
     <row r="38" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
@@ -9676,7 +9708,7 @@
       </c>
     </row>
     <row r="39" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
@@ -9938,7 +9970,7 @@
       </c>
     </row>
     <row r="40" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
@@ -10200,7 +10232,7 @@
       </c>
     </row>
     <row r="41" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
@@ -10462,7 +10494,7 @@
       </c>
     </row>
     <row r="42" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -10724,7 +10756,7 @@
       </c>
     </row>
     <row r="43" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -10986,7 +11018,7 @@
       </c>
     </row>
     <row r="44" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
@@ -11248,7 +11280,7 @@
       </c>
     </row>
     <row r="45" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
@@ -11510,7 +11542,7 @@
       </c>
     </row>
     <row r="46" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
@@ -11772,7 +11804,7 @@
       </c>
     </row>
     <row r="47" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
@@ -12034,7 +12066,7 @@
       </c>
     </row>
     <row r="48" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
@@ -12296,7 +12328,7 @@
       </c>
     </row>
     <row r="49" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
@@ -12558,7 +12590,7 @@
       </c>
     </row>
     <row r="50" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
@@ -12820,7 +12852,7 @@
       </c>
     </row>
     <row r="51" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
@@ -13082,7 +13114,7 @@
       </c>
     </row>
     <row r="52" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
@@ -13344,7 +13376,7 @@
       </c>
     </row>
     <row r="53" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
@@ -13606,7 +13638,7 @@
       </c>
     </row>
     <row r="54" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
@@ -13868,7 +13900,7 @@
       </c>
     </row>
     <row r="55" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
@@ -14130,7 +14162,7 @@
       </c>
     </row>
     <row r="56" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
@@ -14392,7 +14424,7 @@
       </c>
     </row>
     <row r="57" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
@@ -14654,7 +14686,7 @@
       </c>
     </row>
     <row r="58" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
@@ -14916,7 +14948,7 @@
       </c>
     </row>
     <row r="59" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C59" s="3">
+      <c r="C59" s="2">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
@@ -15178,7 +15210,7 @@
       </c>
     </row>
     <row r="60" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
@@ -15440,7 +15472,7 @@
       </c>
     </row>
     <row r="61" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
@@ -15702,7 +15734,7 @@
       </c>
     </row>
     <row r="62" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C62" s="3">
+      <c r="C62" s="2">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
@@ -15964,7 +15996,7 @@
       </c>
     </row>
     <row r="63" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
@@ -16226,7 +16258,7 @@
       </c>
     </row>
     <row r="64" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
@@ -16488,7 +16520,7 @@
       </c>
     </row>
     <row r="65" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C65" s="3">
+      <c r="C65" s="2">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
@@ -16750,7 +16782,7 @@
       </c>
     </row>
     <row r="66" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C66" s="3">
+      <c r="C66" s="2">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
@@ -17012,7 +17044,7 @@
       </c>
     </row>
     <row r="67" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C67" s="3">
+      <c r="C67" s="2">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
@@ -17274,7 +17306,7 @@
       </c>
     </row>
     <row r="68" spans="3:67" x14ac:dyDescent="0.35">
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
@@ -17549,288 +17581,620 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79230DCC-5E5F-492F-8E29-85439474ACBD}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="13.6328125" customWidth="1"/>
     <col min="4" max="5" width="13.6328125" customWidth="1"/>
+    <col min="7" max="8" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="8"/>
+    <col min="13" max="13" width="18.1796875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="14"/>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>128</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3">
+        <v>192</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3">
         <v>0.16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>32</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>5</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="E5" s="5"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>600</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>$B$2 * POWER((A7 - $A$7) / 200, $B$3) +$B$4</f>
         <v>32</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
+        <v>55</v>
+      </c>
+      <c r="G7">
+        <v>600</v>
+      </c>
+      <c r="H7" s="4">
+        <f>$H$2 * POWER(($G$17 - G7) / 200, $H$3) +$H$4</f>
+        <v>341.22776601683825</v>
+      </c>
+      <c r="J7">
+        <v>600</v>
+      </c>
+      <c r="K7" s="4">
+        <f>$K$2 * POWER((J$17 - J7) / 200, $K$3) +$K$4</f>
         <v>21</v>
       </c>
+      <c r="L7" s="8">
+        <f>(K7 *100) / 128</f>
+        <v>16.40625</v>
+      </c>
+      <c r="M7" s="17">
+        <f xml:space="preserve"> 128 / K7</f>
+        <v>6.0952380952380949</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ref="A8:A17" si="0">A7 + 200</f>
         <v>800</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
-        <v>160</v>
+        <v>224</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
         <v>800</v>
       </c>
-      <c r="E8" s="5">
-        <f t="shared" ref="E8:E17" si="3">$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
+      <c r="E8" s="4">
+        <f>$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
+        <v>45.5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G17" si="3">G7 + 200</f>
+        <v>800</v>
+      </c>
+      <c r="H8" s="4">
+        <f>$H$2 * POWER(($G$17 - G8) / 200, $H$3) +$H$4</f>
+        <v>268.00000000000017</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J17" si="4">J7 + 200</f>
+        <v>800</v>
+      </c>
+      <c r="K8" s="4">
+        <f>$K$2 * POWER((J$17 - J8) / 200, $K$3) +$K$4</f>
         <v>17.96</v>
       </c>
+      <c r="L8" s="8">
+        <f t="shared" ref="L8:L17" si="5">(K8 *100) / 128</f>
+        <v>14.03125</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" ref="M8:M17" si="6" xml:space="preserve"> 128 / K8</f>
+        <v>7.1269487750556788</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="B9" s="5">
-        <f t="shared" si="1"/>
-        <v>2080</v>
+      <c r="B9" s="4">
+        <f t="shared" si="1"/>
+        <v>3104</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
+        <f>$E$2 * POWER(($D$17 - D9) / 200, $E$3) +$E$4</f>
+        <v>37</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="H9" s="4">
+        <f>$H$2 * POWER(($G$17 - G9) / 200, $H$3) +$H$4</f>
+        <v>206.01933598375612</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1000</v>
+      </c>
+      <c r="K9" s="4">
+        <f>$K$2 * POWER((J$17 - J9) / 200, $K$3) +$K$4</f>
         <v>15.24</v>
       </c>
+      <c r="L9" s="8">
+        <f t="shared" si="5"/>
+        <v>11.90625</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="6"/>
+        <v>8.3989501312335957</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="B10" s="5">
-        <f t="shared" si="1"/>
-        <v>10400</v>
+      <c r="B10" s="4">
+        <f t="shared" si="1"/>
+        <v>15584</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
+        <f>$E$2 * POWER(($D$17 - D10) / 200, $E$3) +$E$4</f>
+        <v>29.5</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="H10" s="4">
+        <f>$H$2 * POWER(($G$17 - G10) / 200, $H$3) +$H$4</f>
+        <v>154.64181424216488</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="K10" s="4">
+        <f>$K$2 * POWER((J$17 - J10) / 200, $K$3) +$K$4</f>
         <v>12.84</v>
       </c>
+      <c r="L10" s="8">
+        <f t="shared" si="5"/>
+        <v>10.03125</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="6"/>
+        <v>9.9688473520249214</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
-      <c r="B11" s="5">
-        <f t="shared" si="1"/>
-        <v>32800</v>
+      <c r="B11" s="4">
+        <f t="shared" si="1"/>
+        <v>49184</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
+        <f>$E$2 * POWER(($D$17 - D11) / 200, $E$3) +$E$4</f>
+        <v>23</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="3"/>
+        <v>1400</v>
+      </c>
+      <c r="H11" s="4">
+        <f>$H$2 * POWER(($G$17 - G11) / 200, $H$3) +$H$4</f>
+        <v>113.18163074019438</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>1400</v>
+      </c>
+      <c r="K11" s="4">
+        <f>$K$2 * POWER((J$17 - J11) / 200, $K$3) +$K$4</f>
         <v>10.76</v>
       </c>
+      <c r="L11" s="8">
+        <f t="shared" si="5"/>
+        <v>8.40625</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="6"/>
+        <v>11.895910780669146</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="B12" s="5">
-        <f t="shared" si="1"/>
-        <v>80032</v>
+      <c r="B12" s="4">
+        <f t="shared" si="1"/>
+        <v>120032</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
+        <f>$E$2 * POWER(($D$17 - D12) / 200, $E$3) +$E$4</f>
+        <v>17.5</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="3"/>
+        <v>1600</v>
+      </c>
+      <c r="H12" s="4">
+        <f>$H$2 * POWER(($G$17 - G12) / 200, $H$3) +$H$4</f>
+        <v>80.901699437494727</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>1600</v>
+      </c>
+      <c r="K12" s="4">
+        <f>$K$2 * POWER((J$17 - J12) / 200, $K$3) +$K$4</f>
         <v>9</v>
       </c>
+      <c r="L12" s="8">
+        <f t="shared" si="5"/>
+        <v>7.03125</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="6"/>
+        <v>14.222222222222221</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
-      <c r="B13" s="5">
-        <f t="shared" si="1"/>
-        <v>165920</v>
+      <c r="B13" s="4">
+        <f t="shared" si="1"/>
+        <v>248864</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
         <v>1800</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
+        <f>$E$2 * POWER(($D$17 - D13) / 200, $E$3) +$E$4</f>
+        <v>13</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+      <c r="H13" s="4">
+        <f>$H$2 * POWER(($G$17 - G13) / 200, $H$3) +$H$4</f>
+        <v>57</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>1800</v>
+      </c>
+      <c r="K13" s="4">
+        <f>$K$2 * POWER((J$17 - J13) / 200, $K$3) +$K$4</f>
         <v>7.5600000000000005</v>
       </c>
+      <c r="L13" s="8">
+        <f t="shared" si="5"/>
+        <v>5.90625</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="6"/>
+        <v>16.93121693121693</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="B14" s="5">
-        <f t="shared" si="1"/>
-        <v>307360</v>
+      <c r="B14" s="4">
+        <f t="shared" si="1"/>
+        <v>461024</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
+        <f>$E$2 * POWER(($D$17 - D14) / 200, $E$3) +$E$4</f>
+        <v>9.5</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="H14" s="4">
+        <f>$H$2 * POWER(($G$17 - G14) / 200, $H$3) +$H$4</f>
+        <v>40.588457268119903</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="K14" s="4">
+        <f>$K$2 * POWER((J$17 - J14) / 200, $K$3) +$K$4</f>
         <v>6.4399999999999995</v>
       </c>
+      <c r="L14" s="8">
+        <f t="shared" si="5"/>
+        <v>5.03125</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" si="6"/>
+        <v>19.87577639751553</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="B15" s="5">
-        <f t="shared" si="1"/>
-        <v>524320</v>
+      <c r="B15" s="4">
+        <f t="shared" si="1"/>
+        <v>786464</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
         <v>2200</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
+        <f>$E$2 * POWER(($D$17 - D15) / 200, $E$3) +$E$4</f>
+        <v>7</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$H$2 * POWER(($G$17 - G15) / 200, $H$3) +$H$4</f>
+        <v>30.65685424949238</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>2200</v>
+      </c>
+      <c r="K15" s="4">
+        <f>$K$2 * POWER((J$17 - J15) / 200, $K$3) +$K$4</f>
         <v>5.64</v>
       </c>
+      <c r="L15" s="8">
+        <f t="shared" si="5"/>
+        <v>4.40625</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" si="6"/>
+        <v>22.695035460992909</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f>A15 + 200</f>
         <v>2400</v>
       </c>
-      <c r="B16" s="5">
-        <f t="shared" si="1"/>
-        <v>839840</v>
+      <c r="B16" s="4">
+        <f t="shared" si="1"/>
+        <v>1259744</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f>D15 + 200</f>
         <v>2400</v>
       </c>
-      <c r="E16" s="5">
-        <f t="shared" si="3"/>
+      <c r="E16" s="4">
+        <f>$E$2 * POWER(($D$17 - D16) / 200, $E$3) +$E$4</f>
+        <v>5.5</v>
+      </c>
+      <c r="G16">
+        <f>G15 + 200</f>
+        <v>2400</v>
+      </c>
+      <c r="H16" s="4">
+        <f>$H$2 * POWER(($G$17 - G16) / 200, $H$3) +$H$4</f>
+        <v>26</v>
+      </c>
+      <c r="J16">
+        <f>J15 + 200</f>
+        <v>2400</v>
+      </c>
+      <c r="K16" s="4">
+        <f>$K$2 * POWER((J$17 - J16) / 200, $K$3) +$K$4</f>
         <v>5.16</v>
       </c>
+      <c r="L16" s="8">
+        <f t="shared" si="5"/>
+        <v>4.03125</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" si="6"/>
+        <v>24.806201550387595</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
-      <c r="B17" s="5">
-        <f t="shared" si="1"/>
-        <v>1280032</v>
+      <c r="B17" s="4">
+        <f t="shared" si="1"/>
+        <v>1920032</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
         <v>2600</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
+        <f>$E$2 * POWER(($D$17 - D17) / 200, $E$3) +$E$4</f>
+        <v>5</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="H17" s="4">
+        <f>$H$2 * POWER(($G$17 - G17) / 200, $H$3) +$H$4</f>
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>2600</v>
+      </c>
+      <c r="K17" s="4">
+        <f>$K$2 * POWER((J$17 - J17) / 200, $K$3) +$K$4</f>
         <v>5</v>
+      </c>
+      <c r="L17" s="8">
+        <f t="shared" si="5"/>
+        <v>3.90625</v>
+      </c>
+      <c r="M17" s="17">
+        <f t="shared" si="6"/>
+        <v>25.6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17838,45 +18202,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4CD39-04D6-4A1F-9AA8-46EE1D516721}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10">
-        <v>1</v>
+      <c r="E1" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2</v>
       </c>
     </row>
@@ -17885,15 +18250,15 @@
         <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>3</v>
+      <c r="E3" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -17901,9 +18266,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B4" s="9">
-        <f t="shared" si="1"/>
-        <v>12</v>
+      <c r="B4" s="8">
+        <f t="shared" si="1"/>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -17911,9 +18276,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="9">
-        <f t="shared" si="1"/>
-        <v>19</v>
+      <c r="B5" s="8">
+        <f t="shared" si="1"/>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -17921,9 +18286,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="9">
-        <f t="shared" si="1"/>
-        <v>28</v>
+      <c r="B6" s="8">
+        <f t="shared" si="1"/>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -17931,9 +18296,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="9">
-        <f t="shared" si="1"/>
-        <v>39</v>
+      <c r="B7" s="8">
+        <f t="shared" si="1"/>
+        <v>626</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -17941,9 +18306,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="9">
-        <f t="shared" si="1"/>
-        <v>52</v>
+      <c r="B8" s="8">
+        <f t="shared" si="1"/>
+        <v>834</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -17951,9 +18316,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="9">
-        <f t="shared" si="1"/>
-        <v>67</v>
+      <c r="B9" s="8">
+        <f t="shared" si="1"/>
+        <v>1074</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -17961,13 +18326,352 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="9">
-        <f t="shared" si="1"/>
-        <v>84</v>
+      <c r="B10" s="8">
+        <f t="shared" si="1"/>
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D75E8BC-3113-4D5F-9721-2C5404FEE815}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.08984375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="10">
+        <v>800</v>
+      </c>
+      <c r="B2" s="12">
+        <f t="shared" ref="B2:B18" si="0">1 / (1 + POWER(10, (-1 * A2 / $D$2)))</f>
+        <v>0.96055077075785666</v>
+      </c>
+      <c r="D2" s="10">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
+        <f>A2 - 100</f>
+        <v>700</v>
+      </c>
+      <c r="B3" s="12">
+        <f t="shared" si="0"/>
+        <v>0.94231980226632672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
+        <f t="shared" ref="A4:A18" si="1">A3 - 100</f>
+        <v>600</v>
+      </c>
+      <c r="B4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.91639692148646656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="B5" s="12">
+        <f t="shared" si="0"/>
+        <v>0.88030353627105185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>0.83149308082614892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="B7" s="12">
+        <f t="shared" si="0"/>
+        <v>0.76802356512493686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" si="0"/>
+        <v>0.68957284718215062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" si="0"/>
+        <v>0.59846216444498745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="B11" s="12">
+        <f t="shared" si="0"/>
+        <v>0.4015378355550126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="10">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="B12" s="12">
+        <f t="shared" si="0"/>
+        <v>0.31042715281784933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
+        <f t="shared" si="1"/>
+        <v>-300</v>
+      </c>
+      <c r="B13" s="12">
+        <f t="shared" si="0"/>
+        <v>0.23197643487506323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <f t="shared" si="1"/>
+        <v>-400</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" si="0"/>
+        <v>0.16850691917385111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="10">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="0"/>
+        <v>0.11969646372894807</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="10">
+        <f t="shared" si="1"/>
+        <v>-600</v>
+      </c>
+      <c r="B16" s="12">
+        <f t="shared" si="0"/>
+        <v>8.3603078513533449E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="10">
+        <f t="shared" si="1"/>
+        <v>-700</v>
+      </c>
+      <c r="B17" s="12">
+        <f t="shared" si="0"/>
+        <v>5.7680197733673291E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
+        <f t="shared" si="1"/>
+        <v>-800</v>
+      </c>
+      <c r="B18" s="12">
+        <f t="shared" si="0"/>
+        <v>3.9449229242143363E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Testing aggressive search params paired with avoiding looking up piece location improvement in Search.IsMoveInDynamicSearchFutile and Search.IsMoveInQuietSearchFutile methods unless necessary.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E82421-EF9A-49C7-B875-71095A1D8307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A83DD6-74C6-4FF0-9C48-ACEAB169D8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1550" windowWidth="29390" windowHeight="18290" activeTab="2" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
+    <workbookView xWindow="4220" yWindow="1610" windowWidth="29390" windowHeight="18290" activeTab="3" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="LateMoveReductions" sheetId="2" r:id="rId1"/>
@@ -18204,8 +18204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4CD39-04D6-4A1F-9AA8-46EE1D516721}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18340,8 +18340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
2727 +/- 13 Elo at bullet chess.  Tapered futility margins between middlegame and endgame.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A83DD6-74C6-4FF0-9C48-ACEAB169D8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88273CDD-2FFA-4D8A-B48D-EEDC997F4788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4220" yWindow="1610" windowWidth="29390" windowHeight="18290" activeTab="3" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
@@ -18202,10 +18202,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4CD39-04D6-4A1F-9AA8-46EE1D516721}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18226,16 +18226,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="8">
-        <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
-        <v>62</v>
+        <f t="shared" ref="B2:B11" si="0">ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -18246,12 +18246,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
-        <v>2</v>
+        <f>A2 + 1</f>
+        <v>1</v>
       </c>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
-        <v>98</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -18262,72 +18262,82 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
+        <f t="shared" ref="A4:A11" si="1">A3 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="8">
-        <f t="shared" si="1"/>
-        <v>158</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="8">
-        <f t="shared" si="1"/>
-        <v>242</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="8">
-        <f t="shared" si="1"/>
-        <v>350</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="8">
-        <f t="shared" si="1"/>
-        <v>482</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <f t="shared" si="1"/>
-        <v>638</v>
+        <v>626</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="8">
-        <f t="shared" si="1"/>
-        <v>818</v>
+        <v>834</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="8">
-        <f t="shared" si="1"/>
-        <v>1022</v>
+      <c r="B11" s="8">
+        <f t="shared" si="0"/>
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
@@ -18341,7 +18351,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Feature/search param tuning (#53)
* Prevented null move and LMR from dropping into quiet search.  Adjusted default null move reduction from 3 to 2 but allow up to 6 based on static score.  Made LMR more aggressive.

* Testing less aggressive null move pruning, LMR, quiet search recaptures-only, futility pruning, and LMP.

* Testing quiet search of recaptures based on distance from horizon excluding checks.

* 2725 +/- 13 Elo at bullet chess.

* 2722 +/- 13 Elo at bullet chess.

* 2720 +/- 13 Elo at bullet chess.  Extended futility and late move pruning margins out to eight ply from search horizon.

* Testing aggressive search params paired with avoiding looking up piece location improvement in Search.IsMoveInDynamicSearchFutile and Search.IsMoveInQuietSearchFutile methods unless necessary.

* 2724 +/- 13 Elo at bullet chess.

* 2727 +/- 13 Elo at bullet chess.  Tapered futility margins between middlegame and endgame.

* Added comment in Eval.GetStaticScore method.
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F997392-B05E-463E-A510-9A6F5700775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88273CDD-2FFA-4D8A-B48D-EEDC997F4788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1550" windowWidth="29390" windowHeight="18290" activeTab="1" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
+    <workbookView xWindow="4220" yWindow="1610" windowWidth="29390" windowHeight="18290" activeTab="3" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="LateMoveReductions" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -106,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -180,6 +179,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -190,8 +191,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,37 +508,37 @@
   <dimension ref="A1:BO68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
       <c r="D1">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2">
         <v>1</v>
       </c>
@@ -797,10 +796,10 @@
       </c>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -17583,7 +17582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79230DCC-5E5F-492F-8E29-85439474ACBD}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -17594,26 +17593,26 @@
     <col min="7" max="8" width="13.6328125" customWidth="1"/>
     <col min="10" max="10" width="13.6328125" customWidth="1"/>
     <col min="12" max="12" width="8.7265625" style="8"/>
-    <col min="13" max="13" width="18.1796875" style="17" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="18"/>
+      <c r="D1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="16"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -17727,7 +17726,7 @@
       <c r="L6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -17743,365 +17742,365 @@
         <v>600</v>
       </c>
       <c r="E7" s="4">
-        <f>$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
+        <f t="shared" ref="E7:E17" si="0">$E$2 * POWER(($D$17 - D7) / 200, $E$3) +$E$4</f>
         <v>55</v>
       </c>
       <c r="G7">
         <v>600</v>
       </c>
       <c r="H7" s="4">
-        <f>$H$2 * POWER(($G$17 - G7) / 200, $H$3) +$H$4</f>
+        <f t="shared" ref="H7:H17" si="1">$H$2 * POWER(($G$17 - G7) / 200, $H$3) +$H$4</f>
         <v>341.22776601683825</v>
       </c>
       <c r="J7">
         <v>600</v>
       </c>
       <c r="K7" s="4">
-        <f>$K$2 * POWER((J$17 - J7) / 200, $K$3) +$K$4</f>
+        <f t="shared" ref="K7:K17" si="2">$K$2 * POWER((J$17 - J7) / 200, $K$3) +$K$4</f>
         <v>21</v>
       </c>
       <c r="L7" s="8">
         <f>(K7 *100) / 128</f>
         <v>16.40625</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="13">
         <f xml:space="preserve"> 128 / K7</f>
         <v>6.0952380952380949</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
-        <f t="shared" ref="A8:A17" si="0">A7 + 200</f>
+        <f t="shared" ref="A8:A17" si="3">A7 + 200</f>
         <v>800</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" ref="B8:B17" si="1">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
+        <f t="shared" ref="B8:B17" si="4">$B$2 * POWER((A8 - $A$7) / 200, $B$3) +$B$4</f>
         <v>224</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D17" si="2">D7 + 200</f>
+        <f t="shared" ref="D8:D17" si="5">D7 + 200</f>
         <v>800</v>
       </c>
       <c r="E8" s="4">
-        <f>$E$2 * POWER(($D$17 - D8) / 200, $E$3) +$E$4</f>
+        <f t="shared" si="0"/>
         <v>45.5</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G17" si="3">G7 + 200</f>
+        <f t="shared" ref="G8:G17" si="6">G7 + 200</f>
         <v>800</v>
       </c>
       <c r="H8" s="4">
-        <f>$H$2 * POWER(($G$17 - G8) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>268.00000000000017</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J17" si="4">J7 + 200</f>
+        <f t="shared" ref="J8:J17" si="7">J7 + 200</f>
         <v>800</v>
       </c>
       <c r="K8" s="4">
-        <f>$K$2 * POWER((J$17 - J8) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>17.96</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L8:L17" si="5">(K8 *100) / 128</f>
+        <f t="shared" ref="L8:L17" si="8">(K8 *100) / 128</f>
         <v>14.03125</v>
       </c>
-      <c r="M8" s="17">
-        <f t="shared" ref="M8:M17" si="6" xml:space="preserve"> 128 / K8</f>
+      <c r="M8" s="13">
+        <f t="shared" ref="M8:M17" si="9" xml:space="preserve"> 128 / K8</f>
         <v>7.1269487750556788</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="B9" s="4">
-        <f t="shared" si="1"/>
-        <v>3104</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>1000</v>
-      </c>
-      <c r="E9" s="4">
-        <f>$E$2 * POWER(($D$17 - D9) / 200, $E$3) +$E$4</f>
-        <v>37</v>
-      </c>
-      <c r="G9">
         <f t="shared" si="3"/>
         <v>1000</v>
       </c>
+      <c r="B9" s="4">
+        <f t="shared" si="4"/>
+        <v>3104</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
       <c r="H9" s="4">
-        <f>$H$2 * POWER(($G$17 - G9) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>206.01933598375612</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="K9" s="4">
-        <f>$K$2 * POWER((J$17 - J9) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>15.24</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11.90625</v>
       </c>
-      <c r="M9" s="17">
-        <f t="shared" si="6"/>
+      <c r="M9" s="13">
+        <f t="shared" si="9"/>
         <v>8.3989501312335957</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="B10" s="4">
-        <f t="shared" si="1"/>
-        <v>15584</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>1200</v>
-      </c>
-      <c r="E10" s="4">
-        <f>$E$2 * POWER(($D$17 - D10) / 200, $E$3) +$E$4</f>
-        <v>29.5</v>
-      </c>
-      <c r="G10">
         <f t="shared" si="3"/>
         <v>1200</v>
       </c>
+      <c r="B10" s="4">
+        <f t="shared" si="4"/>
+        <v>15584</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="5"/>
+        <v>1200</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>29.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="6"/>
+        <v>1200</v>
+      </c>
       <c r="H10" s="4">
-        <f>$H$2 * POWER(($G$17 - G10) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>154.64181424216488</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1200</v>
       </c>
       <c r="K10" s="4">
-        <f>$K$2 * POWER((J$17 - J10) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>12.84</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10.03125</v>
       </c>
-      <c r="M10" s="17">
-        <f t="shared" si="6"/>
+      <c r="M10" s="13">
+        <f t="shared" si="9"/>
         <v>9.9688473520249214</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="1"/>
-        <v>49184</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>1400</v>
-      </c>
-      <c r="E11" s="4">
-        <f>$E$2 * POWER(($D$17 - D11) / 200, $E$3) +$E$4</f>
-        <v>23</v>
-      </c>
-      <c r="G11">
         <f t="shared" si="3"/>
         <v>1400</v>
       </c>
+      <c r="B11" s="4">
+        <f t="shared" si="4"/>
+        <v>49184</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="5"/>
+        <v>1400</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="6"/>
+        <v>1400</v>
+      </c>
       <c r="H11" s="4">
-        <f>$H$2 * POWER(($G$17 - G11) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>113.18163074019438</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1400</v>
       </c>
       <c r="K11" s="4">
-        <f>$K$2 * POWER((J$17 - J11) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>10.76</v>
       </c>
       <c r="L11" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.40625</v>
       </c>
-      <c r="M11" s="17">
-        <f t="shared" si="6"/>
+      <c r="M11" s="13">
+        <f t="shared" si="9"/>
         <v>11.895910780669146</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="B12" s="4">
-        <f t="shared" si="1"/>
-        <v>120032</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>1600</v>
-      </c>
-      <c r="E12" s="4">
-        <f>$E$2 * POWER(($D$17 - D12) / 200, $E$3) +$E$4</f>
-        <v>17.5</v>
-      </c>
-      <c r="G12">
         <f t="shared" si="3"/>
         <v>1600</v>
       </c>
+      <c r="B12" s="4">
+        <f t="shared" si="4"/>
+        <v>120032</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="5"/>
+        <v>1600</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="6"/>
+        <v>1600</v>
+      </c>
       <c r="H12" s="4">
-        <f>$H$2 * POWER(($G$17 - G12) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>80.901699437494727</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1600</v>
       </c>
       <c r="K12" s="4">
-        <f>$K$2 * POWER((J$17 - J12) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L12" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.03125</v>
       </c>
-      <c r="M12" s="17">
-        <f t="shared" si="6"/>
+      <c r="M12" s="13">
+        <f t="shared" si="9"/>
         <v>14.222222222222221</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="B13" s="4">
-        <f t="shared" si="1"/>
-        <v>248864</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="E13" s="4">
-        <f>$E$2 * POWER(($D$17 - D13) / 200, $E$3) +$E$4</f>
-        <v>13</v>
-      </c>
-      <c r="G13">
         <f t="shared" si="3"/>
         <v>1800</v>
       </c>
+      <c r="B13" s="4">
+        <f t="shared" si="4"/>
+        <v>248864</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="5"/>
+        <v>1800</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="6"/>
+        <v>1800</v>
+      </c>
       <c r="H13" s="4">
-        <f>$H$2 * POWER(($G$17 - G13) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1800</v>
       </c>
       <c r="K13" s="4">
-        <f>$K$2 * POWER((J$17 - J13) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>7.5600000000000005</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.90625</v>
       </c>
-      <c r="M13" s="17">
-        <f t="shared" si="6"/>
+      <c r="M13" s="13">
+        <f t="shared" si="9"/>
         <v>16.93121693121693</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" si="1"/>
-        <v>461024</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>2000</v>
-      </c>
-      <c r="E14" s="4">
-        <f>$E$2 * POWER(($D$17 - D14) / 200, $E$3) +$E$4</f>
-        <v>9.5</v>
-      </c>
-      <c r="G14">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
+      <c r="B14" s="4">
+        <f t="shared" si="4"/>
+        <v>461024</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>2000</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
       <c r="H14" s="4">
-        <f>$H$2 * POWER(($G$17 - G14) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>40.588457268119903</v>
       </c>
       <c r="J14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2000</v>
       </c>
       <c r="K14" s="4">
-        <f>$K$2 * POWER((J$17 - J14) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>6.4399999999999995</v>
       </c>
       <c r="L14" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.03125</v>
       </c>
-      <c r="M14" s="17">
-        <f t="shared" si="6"/>
+      <c r="M14" s="13">
+        <f t="shared" si="9"/>
         <v>19.87577639751553</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>2200</v>
-      </c>
-      <c r="B15" s="4">
-        <f t="shared" si="1"/>
-        <v>786464</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>2200</v>
-      </c>
-      <c r="E15" s="4">
-        <f>$E$2 * POWER(($D$17 - D15) / 200, $E$3) +$E$4</f>
-        <v>7</v>
-      </c>
-      <c r="G15">
         <f t="shared" si="3"/>
         <v>2200</v>
       </c>
+      <c r="B15" s="4">
+        <f t="shared" si="4"/>
+        <v>786464</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>2200</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="6"/>
+        <v>2200</v>
+      </c>
       <c r="H15" s="4">
-        <f>$H$2 * POWER(($G$17 - G15) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>30.65685424949238</v>
       </c>
       <c r="J15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2200</v>
       </c>
       <c r="K15" s="4">
-        <f>$K$2 * POWER((J$17 - J15) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>5.64</v>
       </c>
       <c r="L15" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.40625</v>
       </c>
-      <c r="M15" s="17">
-        <f t="shared" si="6"/>
+      <c r="M15" s="13">
+        <f t="shared" si="9"/>
         <v>22.695035460992909</v>
       </c>
     </row>
@@ -18111,7 +18110,7 @@
         <v>2400</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1259744</v>
       </c>
       <c r="D16">
@@ -18119,7 +18118,7 @@
         <v>2400</v>
       </c>
       <c r="E16" s="4">
-        <f>$E$2 * POWER(($D$17 - D16) / 200, $E$3) +$E$4</f>
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
       <c r="G16">
@@ -18127,7 +18126,7 @@
         <v>2400</v>
       </c>
       <c r="H16" s="4">
-        <f>$H$2 * POWER(($G$17 - G16) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J16">
@@ -18135,57 +18134,57 @@
         <v>2400</v>
       </c>
       <c r="K16" s="4">
-        <f>$K$2 * POWER((J$17 - J16) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>5.16</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.03125</v>
       </c>
-      <c r="M16" s="17">
-        <f t="shared" si="6"/>
+      <c r="M16" s="13">
+        <f t="shared" si="9"/>
         <v>24.806201550387595</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>2600</v>
-      </c>
-      <c r="B17" s="4">
-        <f t="shared" si="1"/>
-        <v>1920032</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>2600</v>
-      </c>
-      <c r="E17" s="4">
-        <f>$E$2 * POWER(($D$17 - D17) / 200, $E$3) +$E$4</f>
-        <v>5</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="3"/>
         <v>2600</v>
       </c>
+      <c r="B17" s="4">
+        <f t="shared" si="4"/>
+        <v>1920032</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="5"/>
+        <v>2600</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>2600</v>
+      </c>
       <c r="H17" s="4">
-        <f>$H$2 * POWER(($G$17 - G17) / 200, $H$3) +$H$4</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="J17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2600</v>
       </c>
       <c r="K17" s="4">
-        <f>$K$2 * POWER((J$17 - J17) / 200, $K$3) +$K$4</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.90625</v>
       </c>
-      <c r="M17" s="17">
-        <f t="shared" si="6"/>
+      <c r="M17" s="13">
+        <f t="shared" si="9"/>
         <v>25.6</v>
       </c>
     </row>
@@ -18203,10 +18202,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4CD39-04D6-4A1F-9AA8-46EE1D516721}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18232,11 +18231,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="8">
-        <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
-        <v>66</v>
+        <f t="shared" ref="B2:B11" si="0">ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -18247,12 +18246,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <f t="shared" ref="A3:A10" si="0">A2 + 1</f>
-        <v>2</v>
+        <f>A2 + 1</f>
+        <v>1</v>
       </c>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
-        <v>114</v>
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -18263,71 +18262,81 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
+        <f t="shared" ref="A4:A11" si="1">A3 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="8">
-        <f t="shared" si="1"/>
-        <v>194</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="8">
-        <f t="shared" si="1"/>
-        <v>306</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="8">
-        <f t="shared" si="1"/>
-        <v>450</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="8">
-        <f t="shared" si="1"/>
-        <v>626</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <f t="shared" si="1"/>
-        <v>834</v>
+        <v>626</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="8">
-        <f t="shared" si="1"/>
-        <v>1074</v>
+        <v>834</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B10" s="8">
-        <f t="shared" si="1"/>
+      <c r="B11" s="8">
+        <f t="shared" si="0"/>
         <v>1346</v>
       </c>
     </row>
@@ -18341,8 +18350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD1855C-969C-4EB8-A34C-AD6D3E0AAD27}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18363,7 +18372,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -18372,7 +18381,7 @@
       </c>
       <c r="B2" s="8">
         <f>ROUNDDOWN(($E$1 * POWER(A2, $E$2)) + $E$3, 0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -18388,7 +18397,7 @@
       </c>
       <c r="B3" s="8">
         <f t="shared" ref="B3:B10" si="1">ROUNDDOWN(($E$1 * POWER(A3, $E$2)) + $E$3, 0)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -18404,7 +18413,7 @@
       </c>
       <c r="B4" s="8">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -18414,7 +18423,7 @@
       </c>
       <c r="B5" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -18424,7 +18433,7 @@
       </c>
       <c r="B6" s="8">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -18434,7 +18443,7 @@
       </c>
       <c r="B7" s="8">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -18444,7 +18453,7 @@
       </c>
       <c r="B8" s="8">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -18454,7 +18463,7 @@
       </c>
       <c r="B9" s="8">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -18464,7 +18473,7 @@
       </c>
       <c r="B10" s="8">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>